<commit_message>
found the duplicate genomes and now removing them
</commit_message>
<xml_diff>
--- a/maf_genomes_list.xlsx
+++ b/maf_genomes_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eklavya/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eklavya/projects/code/BioDragao/africanum_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA84900D-CF63-7A46-AA2C-9506B1B4E1F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511C6CFA-981C-1143-BDFE-A744290C52FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{AF0B711D-CFCC-46BF-8CF3-EDE28DBB3305}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{AF0B711D-CFCC-46BF-8CF3-EDE28DBB3305}"/>
   </bookViews>
   <sheets>
     <sheet name="paired" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="single" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2987,10 +2986,10 @@
     <t>Abhi have downloaded and it is in another folder. We must rename all of them for the Sample_Accession name</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Duplicated genomes - mentioned twice</t>
   </si>
 </sst>
 </file>
@@ -3041,7 +3040,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3060,6 +3059,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3075,7 +3080,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -3087,6 +3092,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3405,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85621DB3-8135-4E18-A5C8-F06E7BAEA16A}">
   <dimension ref="A1:T307"/>
   <sheetViews>
-    <sheetView topLeftCell="A282" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A266" sqref="A266:B267"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3615,7 +3622,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" s="3" customFormat="1">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="12" t="s">
         <v>561</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -3967,7 +3974,7 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="12" t="s">
         <v>561</v>
       </c>
       <c r="B68" t="s">
@@ -5424,7 +5431,7 @@
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="10" t="s">
+      <c r="A114" s="11" t="s">
         <v>754</v>
       </c>
       <c r="B114" t="s">
@@ -6827,7 +6834,7 @@
       </c>
     </row>
     <row r="264" spans="1:20">
-      <c r="A264" t="s">
+      <c r="A264" s="11" t="s">
         <v>610</v>
       </c>
       <c r="B264" t="s">
@@ -6843,7 +6850,7 @@
       </c>
     </row>
     <row r="266" spans="1:20">
-      <c r="A266" t="s">
+      <c r="A266" s="11" t="s">
         <v>611</v>
       </c>
       <c r="B266" t="s">
@@ -6851,7 +6858,7 @@
       </c>
     </row>
     <row r="267" spans="1:20">
-      <c r="A267" t="s">
+      <c r="A267" s="11" t="s">
         <v>612</v>
       </c>
       <c r="B267" t="s">
@@ -7135,7 +7142,7 @@
       </c>
     </row>
     <row r="274" spans="1:16" s="4" customFormat="1">
-      <c r="A274" s="4" t="s">
+      <c r="A274" s="11" t="s">
         <v>754</v>
       </c>
       <c r="B274" s="4" t="s">
@@ -7971,7 +7978,7 @@
       </c>
     </row>
     <row r="293" spans="1:20" s="4" customFormat="1">
-      <c r="A293" s="4" t="s">
+      <c r="A293" s="11" t="s">
         <v>611</v>
       </c>
       <c r="B293" s="4" t="s">
@@ -8103,7 +8110,7 @@
       </c>
     </row>
     <row r="296" spans="1:20" s="4" customFormat="1">
-      <c r="A296" s="4" t="s">
+      <c r="A296" s="11" t="s">
         <v>612</v>
       </c>
       <c r="B296" s="4" t="s">
@@ -8191,7 +8198,7 @@
       </c>
     </row>
     <row r="298" spans="1:20" s="4" customFormat="1">
-      <c r="A298" s="4" t="s">
+      <c r="A298" s="11" t="s">
         <v>610</v>
       </c>
       <c r="B298" s="4" t="s">
@@ -8362,11 +8369,11 @@
       </c>
     </row>
     <row r="307" spans="1:2">
-      <c r="A307" s="6" t="s">
+      <c r="A307" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="B307" t="s">
         <v>985</v>
-      </c>
-      <c r="B307" t="s">
-        <v>986</v>
       </c>
     </row>
   </sheetData>
@@ -9241,7 +9248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD0721F-57A9-C54D-A3E5-9829E8E841D6}">
   <dimension ref="A1:B208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+    <sheetView topLeftCell="A193" workbookViewId="0">
       <selection activeCell="C217" sqref="C217"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working on creating the structure of final python files
</commit_message>
<xml_diff>
--- a/maf_genomes_list.xlsx
+++ b/maf_genomes_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eklavya/projects/code/BioDragao/africanum_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511C6CFA-981C-1143-BDFE-A744290C52FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866A5805-F74B-2647-8431-B4B105630182}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{AF0B711D-CFCC-46BF-8CF3-EDE28DBB3305}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="988">
   <si>
     <t>ERR702401</t>
   </si>
@@ -2977,12 +2977,6 @@
     <t>SAMEA2535035</t>
   </si>
   <si>
-    <t>Ok in the folder maf-genomes</t>
-  </si>
-  <si>
-    <t>we must download</t>
-  </si>
-  <si>
     <t>Abhi have downloaded and it is in another folder. We must rename all of them for the Sample_Accession name</t>
   </si>
   <si>
@@ -2990,6 +2984,15 @@
   </si>
   <si>
     <t xml:space="preserve">  Duplicated genomes - mentioned twice</t>
+  </si>
+  <si>
+    <t>Missing - abhi folder</t>
+  </si>
+  <si>
+    <t>we must download - ena</t>
+  </si>
+  <si>
+    <t>Ok in the folder maf-genomes - em</t>
   </si>
 </sst>
 </file>
@@ -3040,7 +3043,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3065,6 +3068,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3080,7 +3089,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -3094,6 +3103,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3410,10 +3421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85621DB3-8135-4E18-A5C8-F06E7BAEA16A}">
-  <dimension ref="A1:T307"/>
+  <dimension ref="A1:T308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A302" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E307" sqref="E307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3838,7 +3849,7 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="13" t="s">
         <v>593</v>
       </c>
       <c r="B51" t="s">
@@ -3862,7 +3873,7 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="13" t="s">
         <v>596</v>
       </c>
       <c r="B54" t="s">
@@ -8355,24 +8366,29 @@
     </row>
     <row r="304" spans="1:20">
       <c r="A304" s="8" t="s">
-        <v>982</v>
+        <v>987</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="A305" s="7" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306" s="6" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307" s="12" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B307" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
+      <c r="A308" s="14" t="s">
         <v>985</v>
       </c>
     </row>

</xml_diff>

<commit_message>
now we have all the genomes
</commit_message>
<xml_diff>
--- a/maf_genomes_list.xlsx
+++ b/maf_genomes_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eklavya/projects/code/BioDragao/africanum_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866A5805-F74B-2647-8431-B4B105630182}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D070921-C99F-DA41-986D-4E9F1FC6F8D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{AF0B711D-CFCC-46BF-8CF3-EDE28DBB3305}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="990">
   <si>
     <t>ERR702401</t>
   </si>
@@ -2993,6 +2993,12 @@
   </si>
   <si>
     <t>Ok in the folder maf-genomes - em</t>
+  </si>
+  <si>
+    <t>ftp://ftp.sra.ebi.ac.uk/vol1/fastq/ERR120/005/ERR1203075/ERR1203075_1.fastq.gz;ftp://ftp.sra.ebi.ac.uk/vol1/fastq/ERR120/005/ERR1203075/ERR1203075_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>ftp://ftp.sra.ebi.ac.uk/vol1/fastq/ERR120/008/ERR1203078/ERR1203078_1.fastq.gz;ftp://ftp.sra.ebi.ac.uk/vol1/fastq/ERR120/008/ERR1203078/ERR1203078_2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -3423,8 +3429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85621DB3-8135-4E18-A5C8-F06E7BAEA16A}">
   <dimension ref="A1:T308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A302" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E307" sqref="E307"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3832,7 +3838,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="3" customFormat="1">
+    <row r="49" spans="1:6" s="3" customFormat="1">
       <c r="A49" s="3" t="s">
         <v>591</v>
       </c>
@@ -3840,7 +3846,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:6">
       <c r="A50" s="10" t="s">
         <v>594</v>
       </c>
@@ -3848,15 +3854,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:6">
       <c r="A51" s="13" t="s">
         <v>593</v>
       </c>
       <c r="B51" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="F51" s="2" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="10" t="s">
         <v>597</v>
       </c>
@@ -3864,7 +3873,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:6">
       <c r="A53" s="10" t="s">
         <v>598</v>
       </c>
@@ -3872,15 +3881,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:6">
       <c r="A54" s="13" t="s">
         <v>596</v>
       </c>
       <c r="B54" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="F54" s="2" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="9" t="s">
         <v>536</v>
       </c>
@@ -3888,7 +3900,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:6">
       <c r="A56" s="9" t="s">
         <v>537</v>
       </c>
@@ -3896,7 +3908,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:6">
       <c r="A57" s="9" t="s">
         <v>539</v>
       </c>
@@ -3904,7 +3916,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:6">
       <c r="A58" s="9" t="s">
         <v>540</v>
       </c>
@@ -3912,7 +3924,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:6">
       <c r="A59" s="9" t="s">
         <v>541</v>
       </c>
@@ -3920,7 +3932,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:6">
       <c r="A60" s="9" t="s">
         <v>542</v>
       </c>
@@ -3928,7 +3940,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:6">
       <c r="A61" s="9" t="s">
         <v>547</v>
       </c>
@@ -3936,7 +3948,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:6">
       <c r="A62" s="9" t="s">
         <v>548</v>
       </c>
@@ -3944,7 +3956,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:6">
       <c r="A63" s="9" t="s">
         <v>549</v>
       </c>
@@ -3952,7 +3964,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:6">
       <c r="A64" s="9" t="s">
         <v>550</v>
       </c>
@@ -8396,8 +8408,12 @@
   <sortState ref="A2:T301">
     <sortCondition ref="B2:B301"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="F51" r:id="rId1" xr:uid="{97903408-E3C7-494C-B899-3B1D7A6EEE6E}"/>
+    <hyperlink ref="F54" r:id="rId2" xr:uid="{0E66A4EF-8195-7647-93FA-359F5FC1CE61}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>